<commit_message>
Adding changes to spreadsheet
</commit_message>
<xml_diff>
--- a/UberCode_FinalProject_TestReport.xlsx
+++ b/UberCode_FinalProject_TestReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markl\Documents\Studies\CSCI443\FinalProject_Reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Addison Boyer\Documents\Spring 2020\User Interface Design\CSCI443\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292906EC-FA52-4C0A-8878-AB1E5409AAF7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC23C7D9-C655-4553-9D58-020905939A68}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10245" yWindow="2190" windowWidth="27000" windowHeight="14160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan Overview" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
   <si>
     <t>Testing Scope</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>Tester: Colton Gareth</t>
+  </si>
+  <si>
+    <t>Multiple attempts to press over arrows in the navigation menu, currently don't do anything.  May be misleading if they don't have a function? Scrolling seems to be an issue, i.e. try to condense the content so more is visible without scrolling.  It's not apparent when you're on the home screen.  Feedback: for someone with mathematical brain easy thing to do, artistic creative thinkers harder.  Look out for the left brain and right brain kind of thinker.  Wasn't very obvious that it's a home screen, I knew where to look but wasn't obvious.  See the logout, maybe user profile picture (or dropdown to verify that you're logged in).  Not lot's of difference.</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -475,31 +478,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1">
@@ -543,24 +521,12 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -594,18 +560,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -626,6 +580,63 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -929,102 +940,102 @@
       <selection activeCell="E15" sqref="E15:F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.83984375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="16.68359375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.88671875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.26171875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.15625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="36.5234375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83984375" style="1"/>
+    <col min="4" max="4" width="13.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="36.5546875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="39" customHeight="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="47"/>
     </row>
     <row r="2" spans="1:6" ht="19.2" customHeight="1">
-      <c r="A2" s="20"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="22.35" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="48">
         <v>1</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
@@ -1048,104 +1059,104 @@
       <c r="A13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="3"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="36" t="s">
+      <c r="C22" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="36" t="s">
+      <c r="D22" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="36" t="s">
+      <c r="E22" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="F22" s="36" t="s">
+      <c r="F22" s="26" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1153,19 +1164,19 @@
       <c r="A23" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B23" s="11">
         <v>43922</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="26">
+      <c r="B24" s="19">
         <v>43957</v>
       </c>
     </row>
@@ -41133,6 +41144,12 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="18">
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B3:F3"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="E18:F18"/>
@@ -41140,12 +41157,6 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B3:F3"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E13:F13"/>
@@ -41164,22 +41175,22 @@
   </sheetPr>
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24:F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.83984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="78.68359375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.41796875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5234375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.15625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.3671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="4.83984375" style="1" customWidth="1"/>
-    <col min="8" max="11" width="8.83984375" style="1"/>
-    <col min="12" max="12" width="3.68359375" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="1" width="15.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="78.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="4.88671875" style="1" customWidth="1"/>
+    <col min="8" max="11" width="8.88671875" style="1"/>
+    <col min="12" max="12" width="3.6640625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -41205,373 +41216,537 @@
       <c r="B3" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="49"/>
-      <c r="H3" s="37" t="s">
+      <c r="G3" s="36"/>
+      <c r="H3" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="38" t="s">
+      <c r="I3" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="J3" s="39" t="s">
+      <c r="J3" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="K3" s="40" t="s">
+      <c r="K3" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="L3" s="49"/>
-      <c r="M3" s="37" t="s">
+      <c r="L3" s="36"/>
+      <c r="M3" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="N3" s="38" t="s">
+      <c r="N3" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="O3" s="39" t="s">
+      <c r="O3" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="P3" s="40" t="s">
+      <c r="P3" s="30" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="21">
+      <c r="A4" s="14">
         <v>1</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="42"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="32"/>
     </row>
     <row r="5" spans="1:16">
       <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="31">
         <v>5</v>
       </c>
-      <c r="D5" s="42">
+      <c r="D5" s="32">
         <v>4</v>
       </c>
-      <c r="E5" s="42">
+      <c r="E5" s="32">
         <v>5</v>
       </c>
-      <c r="F5" s="43">
+      <c r="F5" s="33">
         <v>4</v>
       </c>
-      <c r="G5" s="42"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="1">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1">
+        <v>4</v>
+      </c>
+      <c r="K5" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:16">
       <c r="B6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="41">
+      <c r="C6" s="31">
         <v>5</v>
       </c>
-      <c r="D6" s="42">
+      <c r="D6" s="32">
         <v>5</v>
       </c>
-      <c r="E6" s="42">
+      <c r="E6" s="32">
         <v>5</v>
       </c>
-      <c r="F6" s="43">
+      <c r="F6" s="33">
         <v>5</v>
       </c>
-      <c r="G6" s="42"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="1">
+        <v>4</v>
+      </c>
+      <c r="I6" s="1">
+        <v>4</v>
+      </c>
+      <c r="J6" s="1">
+        <v>5</v>
+      </c>
+      <c r="K6" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:16">
       <c r="B7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="31">
         <v>5</v>
       </c>
-      <c r="D7" s="42">
+      <c r="D7" s="32">
         <v>5</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="32">
         <v>5</v>
       </c>
-      <c r="F7" s="43">
+      <c r="F7" s="33">
         <v>4</v>
       </c>
-      <c r="G7" s="42"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="1">
+        <v>5</v>
+      </c>
+      <c r="I7" s="1">
+        <v>4</v>
+      </c>
+      <c r="J7" s="1">
+        <v>4</v>
+      </c>
+      <c r="K7" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:16">
       <c r="B8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="31">
         <v>5</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D8" s="32">
         <v>4</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="32">
         <v>5</v>
       </c>
-      <c r="F8" s="43">
+      <c r="F8" s="33">
         <v>4</v>
       </c>
-      <c r="G8" s="42"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="1">
+        <v>5</v>
+      </c>
+      <c r="I8" s="1">
+        <v>5</v>
+      </c>
+      <c r="J8" s="1">
+        <v>5</v>
+      </c>
+      <c r="K8" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:16">
       <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="41">
+      <c r="C9" s="31">
         <v>3</v>
       </c>
-      <c r="D9" s="42">
+      <c r="D9" s="32">
         <v>4</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="32">
         <v>4</v>
       </c>
-      <c r="F9" s="43">
+      <c r="F9" s="33">
         <v>3</v>
       </c>
-      <c r="G9" s="42"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="1">
+        <v>5</v>
+      </c>
+      <c r="I9" s="1">
+        <v>4</v>
+      </c>
+      <c r="J9" s="1">
+        <v>3</v>
+      </c>
+      <c r="K9" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="C10" s="41"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="42"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="32"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="21">
+      <c r="A11" s="14">
         <v>2</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="42"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="32"/>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="22"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="41">
+      <c r="C12" s="31">
         <v>5</v>
       </c>
-      <c r="D12" s="42">
+      <c r="D12" s="32">
         <v>4</v>
       </c>
-      <c r="E12" s="42">
+      <c r="E12" s="32">
         <v>5</v>
       </c>
-      <c r="F12" s="43">
+      <c r="F12" s="33">
         <v>3</v>
       </c>
-      <c r="G12" s="42"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="1">
+        <v>5</v>
+      </c>
+      <c r="I12" s="1">
+        <v>5</v>
+      </c>
+      <c r="J12" s="1">
+        <v>5</v>
+      </c>
+      <c r="K12" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="22"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="41">
+      <c r="C13" s="31">
         <v>4</v>
       </c>
-      <c r="D13" s="42">
+      <c r="D13" s="32">
         <v>5</v>
       </c>
-      <c r="E13" s="42">
+      <c r="E13" s="32">
         <v>4</v>
       </c>
-      <c r="F13" s="43">
+      <c r="F13" s="33">
         <v>2</v>
       </c>
-      <c r="G13" s="42"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="1">
+        <v>5</v>
+      </c>
+      <c r="I13" s="1">
+        <v>3</v>
+      </c>
+      <c r="J13" s="1">
+        <v>5</v>
+      </c>
+      <c r="K13" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="22"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="41">
+      <c r="C14" s="31">
         <v>3</v>
       </c>
-      <c r="D14" s="42">
+      <c r="D14" s="32">
         <v>2</v>
       </c>
-      <c r="E14" s="42">
+      <c r="E14" s="32">
         <v>2</v>
       </c>
-      <c r="F14" s="43">
+      <c r="F14" s="33">
         <v>1</v>
       </c>
-      <c r="G14" s="42"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="1">
+        <v>5</v>
+      </c>
+      <c r="I14" s="1">
+        <v>4</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1</v>
+      </c>
+      <c r="K14" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:16">
-      <c r="C15" s="41"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="42"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="32"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="21">
+      <c r="A16" s="14">
         <v>3</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="42"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="32"/>
     </row>
     <row r="17" spans="2:13">
       <c r="B17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="41">
+      <c r="C17" s="31">
         <v>5</v>
       </c>
-      <c r="D17" s="42">
+      <c r="D17" s="32">
         <v>4</v>
       </c>
-      <c r="E17" s="42">
+      <c r="E17" s="32">
         <v>5</v>
       </c>
-      <c r="F17" s="43">
+      <c r="F17" s="33">
         <v>3</v>
       </c>
-      <c r="G17" s="42"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="1">
+        <v>5</v>
+      </c>
+      <c r="I17" s="1">
+        <v>5</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1</v>
+      </c>
+      <c r="K17" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="18" spans="2:13">
       <c r="B18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="41">
+      <c r="C18" s="31">
         <v>5</v>
       </c>
-      <c r="D18" s="42">
+      <c r="D18" s="32">
         <v>4</v>
       </c>
-      <c r="E18" s="42">
+      <c r="E18" s="32">
         <v>5</v>
       </c>
-      <c r="F18" s="43">
+      <c r="F18" s="33">
         <v>2</v>
       </c>
-      <c r="G18" s="42"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="1">
+        <v>5</v>
+      </c>
+      <c r="I18" s="1">
+        <v>3</v>
+      </c>
+      <c r="J18" s="1">
+        <v>2</v>
+      </c>
+      <c r="K18" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="2:13">
       <c r="B19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="41">
+      <c r="C19" s="31">
         <v>4</v>
       </c>
-      <c r="D19" s="42">
+      <c r="D19" s="32">
         <v>3</v>
       </c>
-      <c r="E19" s="42">
+      <c r="E19" s="32">
         <v>4</v>
       </c>
-      <c r="F19" s="43">
+      <c r="F19" s="33">
         <v>1</v>
       </c>
-      <c r="G19" s="42"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="1">
+        <v>5</v>
+      </c>
+      <c r="I19" s="1">
+        <v>4</v>
+      </c>
+      <c r="J19" s="1">
+        <v>2</v>
+      </c>
+      <c r="K19" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="20" spans="2:13">
       <c r="B20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="41">
+      <c r="C20" s="31">
         <v>4</v>
       </c>
-      <c r="D20" s="42">
+      <c r="D20" s="32">
         <v>4</v>
       </c>
-      <c r="E20" s="42">
+      <c r="E20" s="32">
         <v>4</v>
       </c>
-      <c r="F20" s="43">
+      <c r="F20" s="33">
         <v>4</v>
       </c>
-      <c r="G20" s="42"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="1">
+        <v>4</v>
+      </c>
+      <c r="I20" s="1">
+        <v>5</v>
+      </c>
+      <c r="J20" s="1">
+        <v>3</v>
+      </c>
+      <c r="K20" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="21" spans="2:13">
       <c r="B21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="41">
+      <c r="C21" s="31">
         <v>5</v>
       </c>
-      <c r="D21" s="42">
+      <c r="D21" s="32">
         <v>5</v>
       </c>
-      <c r="E21" s="42">
+      <c r="E21" s="32">
         <v>4</v>
       </c>
-      <c r="F21" s="43">
+      <c r="F21" s="33">
         <v>4</v>
       </c>
-      <c r="G21" s="42"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="1">
+        <v>4</v>
+      </c>
+      <c r="I21" s="1">
+        <v>4</v>
+      </c>
+      <c r="J21" s="1">
+        <v>5</v>
+      </c>
+      <c r="K21" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="2:13">
-      <c r="C22" s="41"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="42"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="32"/>
     </row>
     <row r="23" spans="2:13">
-      <c r="C23" s="44" t="s">
+      <c r="C23" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="44" t="s">
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="M23" s="44" t="s">
+      <c r="M23" s="34" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="24" spans="2:13" ht="193.5" customHeight="1">
-      <c r="B24" s="29"/>
-      <c r="C24" s="45" t="s">
+      <c r="B24" s="22"/>
+      <c r="C24" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="46"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="48"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="56" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" s="55"/>
+      <c r="I24" s="55"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="55"/>
+      <c r="L24" s="55"/>
     </row>
     <row r="25" spans="2:13">
-      <c r="C25" s="28"/>
+      <c r="C25" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C24:F24"/>
+    <mergeCell ref="G24:L24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -41584,22 +41759,22 @@
   </sheetPr>
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.83984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="78.68359375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.41796875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5234375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.15625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.3671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="4.83984375" style="1" customWidth="1"/>
-    <col min="8" max="11" width="8.83984375" style="1"/>
-    <col min="12" max="12" width="3.68359375" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="1" width="15.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="78.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="4.88671875" style="1" customWidth="1"/>
+    <col min="8" max="11" width="8.88671875" style="1"/>
+    <col min="12" max="12" width="3.6640625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -41619,226 +41794,226 @@
       </c>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="54" t="s">
+      <c r="F3" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="49"/>
-      <c r="H3" s="51" t="s">
+      <c r="G3" s="36"/>
+      <c r="H3" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="52" t="s">
+      <c r="I3" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="J3" s="53" t="s">
+      <c r="J3" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="K3" s="54" t="s">
+      <c r="K3" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="L3" s="49"/>
-      <c r="M3" s="51" t="s">
+      <c r="L3" s="36"/>
+      <c r="M3" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="N3" s="52" t="s">
+      <c r="N3" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="O3" s="53" t="s">
+      <c r="O3" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="P3" s="54" t="s">
+      <c r="P3" s="41" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="21">
+      <c r="A4" s="14">
         <v>1</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="42"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="32"/>
     </row>
     <row r="5" spans="1:16">
-      <c r="C5" s="41"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="42"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="32"/>
     </row>
     <row r="6" spans="1:16">
-      <c r="C6" s="41"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="42"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="32"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="C7" s="41"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="42"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="32"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="C8" s="41"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="42"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="32"/>
     </row>
     <row r="9" spans="1:16">
-      <c r="C9" s="41"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="42"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="32"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="C10" s="41"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="42"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="32"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="21">
+      <c r="A11" s="14">
         <v>2</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="42"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="32"/>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="22"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="42"/>
+      <c r="A12" s="15"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="32"/>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="22"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="42"/>
+      <c r="A13" s="15"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="32"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="22"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="42"/>
+      <c r="A14" s="15"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="32"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="C15" s="41"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="42"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="32"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="21">
+      <c r="A16" s="14">
         <v>3</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="42"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="32"/>
     </row>
     <row r="17" spans="2:13">
-      <c r="C17" s="41"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="42"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="32"/>
     </row>
     <row r="18" spans="2:13">
-      <c r="C18" s="41"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="42"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="32"/>
     </row>
     <row r="19" spans="2:13">
-      <c r="C19" s="41"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="42"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="32"/>
     </row>
     <row r="20" spans="2:13">
-      <c r="C20" s="41"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="42"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="32"/>
     </row>
     <row r="21" spans="2:13">
-      <c r="C21" s="41"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="42"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="32"/>
     </row>
     <row r="22" spans="2:13">
-      <c r="C22" s="41"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="42"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="32"/>
     </row>
     <row r="23" spans="2:13">
-      <c r="C23" s="44" t="s">
+      <c r="C23" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="44" t="s">
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="M23" s="44" t="s">
+      <c r="M23" s="34" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="24" spans="2:13" ht="193.5" customHeight="1">
-      <c r="B24" s="29"/>
-      <c r="C24" s="45" t="s">
+      <c r="B24" s="22"/>
+      <c r="C24" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="46"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="48"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="35"/>
     </row>
     <row r="25" spans="2:13">
-      <c r="C25" s="28"/>
+      <c r="C25" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Update with my first round of tests.
</commit_message>
<xml_diff>
--- a/UberCode_FinalProject_TestReport.xlsx
+++ b/UberCode_FinalProject_TestReport.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Addison Boyer\Documents\Spring 2020\User Interface Design\CSCI443\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colton\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC23C7D9-C655-4553-9D58-020905939A68}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10245" yWindow="2190" windowWidth="27000" windowHeight="14160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Testing Round #1 " sheetId="3" r:id="rId2"/>
     <sheet name="Testing Round #2" sheetId="10" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="60">
   <si>
     <t>Testing Scope</t>
   </si>
@@ -211,11 +210,14 @@
   <si>
     <t>Multiple attempts to press over arrows in the navigation menu, currently don't do anything.  May be misleading if they don't have a function? Scrolling seems to be an issue, i.e. try to condense the content so more is visible without scrolling.  It's not apparent when you're on the home screen.  Feedback: for someone with mathematical brain easy thing to do, artistic creative thinkers harder.  Look out for the left brain and right brain kind of thinker.  Wasn't very obvious that it's a home screen, I knew where to look but wasn't obvious.  See the logout, maybe user profile picture (or dropdown to verify that you're logged in).  Not lot's of difference.</t>
   </si>
+  <si>
+    <t>The initial wave of testing went well, although limitations of feedback from the hardware of AdobeXD make some navigation difficult, namely due to the lacking of a scroll bar or feedback of hovering over buttons. Once the users got a feel for how the buttons worked and learned that they were a drop down menu, navigating the webpage to view the competitve streams was much more efficient. They also didnt find the home page button of &lt;U.C&gt; to be very intutitive.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -450,7 +452,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -582,14 +584,6 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -615,6 +609,14 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -631,12 +633,16 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -929,7 +935,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF43A666"/>
     <pageSetUpPr fitToPage="1"/>
@@ -940,28 +946,28 @@
       <selection activeCell="E15" sqref="E15:F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="36.5546875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="13.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="36.5703125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="39" customHeight="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="47"/>
-    </row>
-    <row r="2" spans="1:6" ht="19.2" customHeight="1">
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="45"/>
+    </row>
+    <row r="2" spans="1:6" ht="19.149999999999999" customHeight="1">
       <c r="A2" s="13"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -973,59 +979,59 @@
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="48">
+      <c r="B5" s="46">
         <v>1</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="4" t="s">
@@ -1059,19 +1065,19 @@
       <c r="A13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
       <c r="E14" s="51"/>
       <c r="F14" s="51"/>
     </row>
@@ -1079,39 +1085,39 @@
       <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="6" t="s">
@@ -41144,12 +41150,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="18">
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B3:F3"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="E18:F18"/>
@@ -41162,6 +41162,12 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="E16:F16"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="93" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -41169,28 +41175,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF2E6AB2"/>
   </sheetPr>
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:F24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24:P24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="78.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="4.88671875" style="1" customWidth="1"/>
-    <col min="8" max="11" width="8.88671875" style="1"/>
-    <col min="12" max="12" width="3.6640625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="78.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" style="1" customWidth="1"/>
+    <col min="8" max="11" width="8.85546875" style="1"/>
+    <col min="12" max="12" width="3.7109375" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -41297,6 +41303,12 @@
       <c r="K5" s="1">
         <v>5</v>
       </c>
+      <c r="M5" s="1">
+        <v>5</v>
+      </c>
+      <c r="N5" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:16">
       <c r="B6" s="1" t="s">
@@ -41327,6 +41339,12 @@
       <c r="K6" s="1">
         <v>5</v>
       </c>
+      <c r="M6" s="1">
+        <v>5</v>
+      </c>
+      <c r="N6" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:16">
       <c r="B7" s="1" t="s">
@@ -41357,6 +41375,12 @@
       <c r="K7" s="1">
         <v>5</v>
       </c>
+      <c r="M7" s="1">
+        <v>5</v>
+      </c>
+      <c r="N7" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:16">
       <c r="B8" s="1" t="s">
@@ -41387,6 +41411,12 @@
       <c r="K8" s="1">
         <v>5</v>
       </c>
+      <c r="M8" s="1">
+        <v>5</v>
+      </c>
+      <c r="N8" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:16">
       <c r="B9" s="1" t="s">
@@ -41415,6 +41445,12 @@
         <v>3</v>
       </c>
       <c r="K9" s="1">
+        <v>5</v>
+      </c>
+      <c r="M9" s="1">
+        <v>5</v>
+      </c>
+      <c r="N9" s="1">
         <v>5</v>
       </c>
     </row>
@@ -41468,6 +41504,12 @@
       <c r="K12" s="1">
         <v>5</v>
       </c>
+      <c r="M12" s="1">
+        <v>5</v>
+      </c>
+      <c r="N12" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="15"/>
@@ -41499,6 +41541,12 @@
       <c r="K13" s="1">
         <v>4</v>
       </c>
+      <c r="M13" s="1">
+        <v>5</v>
+      </c>
+      <c r="N13" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="15"/>
@@ -41530,6 +41578,12 @@
       <c r="K14" s="1">
         <v>5</v>
       </c>
+      <c r="M14" s="1">
+        <v>5</v>
+      </c>
+      <c r="N14" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:16">
       <c r="C15" s="31"/>
@@ -41551,7 +41605,7 @@
       <c r="F16" s="33"/>
       <c r="G16" s="32"/>
     </row>
-    <row r="17" spans="2:13">
+    <row r="17" spans="2:16">
       <c r="B17" s="1" t="s">
         <v>41</v>
       </c>
@@ -41580,8 +41634,14 @@
       <c r="K17" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="2:13">
+      <c r="M17" s="1">
+        <v>5</v>
+      </c>
+      <c r="N17" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16">
       <c r="B18" s="1" t="s">
         <v>42</v>
       </c>
@@ -41610,8 +41670,14 @@
       <c r="K18" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="2:13">
+      <c r="M18" s="1">
+        <v>3</v>
+      </c>
+      <c r="N18" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16">
       <c r="B19" s="1" t="s">
         <v>43</v>
       </c>
@@ -41640,8 +41706,14 @@
       <c r="K19" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="2:13">
+      <c r="M19" s="1">
+        <v>3</v>
+      </c>
+      <c r="N19" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16">
       <c r="B20" s="1" t="s">
         <v>44</v>
       </c>
@@ -41670,8 +41742,14 @@
       <c r="K20" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="2:13">
+      <c r="M20" s="1">
+        <v>3</v>
+      </c>
+      <c r="N20" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16">
       <c r="B21" s="1" t="s">
         <v>45</v>
       </c>
@@ -41700,15 +41778,21 @@
       <c r="K21" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="2:13">
+      <c r="M21" s="1">
+        <v>4</v>
+      </c>
+      <c r="N21" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16">
       <c r="C22" s="31"/>
       <c r="D22" s="32"/>
       <c r="E22" s="32"/>
       <c r="F22" s="33"/>
       <c r="G22" s="32"/>
     </row>
-    <row r="23" spans="2:13">
+    <row r="23" spans="2:16">
       <c r="C23" s="34" t="s">
         <v>53</v>
       </c>
@@ -41723,7 +41807,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="2:13" ht="193.5" customHeight="1">
+    <row r="24" spans="2:16" ht="193.5" customHeight="1">
       <c r="B24" s="22"/>
       <c r="C24" s="52" t="s">
         <v>54</v>
@@ -41731,29 +41815,36 @@
       <c r="D24" s="53"/>
       <c r="E24" s="53"/>
       <c r="F24" s="54"/>
-      <c r="G24" s="56" t="s">
+      <c r="G24" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="H24" s="55"/>
-      <c r="I24" s="55"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="55"/>
-      <c r="L24" s="55"/>
-    </row>
-    <row r="25" spans="2:13">
+      <c r="H24" s="56"/>
+      <c r="I24" s="56"/>
+      <c r="J24" s="56"/>
+      <c r="K24" s="56"/>
+      <c r="L24" s="56"/>
+      <c r="M24" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="N24" s="57"/>
+      <c r="O24" s="57"/>
+      <c r="P24" s="57"/>
+    </row>
+    <row r="25" spans="2:16">
       <c r="C25" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C24:F24"/>
     <mergeCell ref="G24:L24"/>
+    <mergeCell ref="M24:P24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02ED60A0-2B3F-4442-A5AD-5BB5F2E76CAB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
@@ -41763,18 +41854,18 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="78.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="4.88671875" style="1" customWidth="1"/>
-    <col min="8" max="11" width="8.88671875" style="1"/>
-    <col min="12" max="12" width="3.6640625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="78.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" style="1" customWidth="1"/>
+    <col min="8" max="11" width="8.85546875" style="1"/>
+    <col min="12" max="12" width="3.7109375" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">

</xml_diff>

<commit_message>
Part 2 test results uploaded
</commit_message>
<xml_diff>
--- a/UberCode_FinalProject_TestReport.xlsx
+++ b/UberCode_FinalProject_TestReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3975" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan Overview" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="69">
   <si>
     <t>Testing Scope</t>
   </si>
@@ -213,12 +213,39 @@
   <si>
     <t>The initial wave of testing went well, although limitations of feedback from the hardware of AdobeXD make some navigation difficult, namely due to the lacking of a scroll bar or feedback of hovering over buttons. Once the users got a feel for how the buttons worked and learned that they were a drop down menu, navigating the webpage to view the competitve streams was much more efficient. They also didnt find the home page button of &lt;U.C&gt; to be very intutitive.</t>
   </si>
+  <si>
+    <t xml:space="preserve"> Select “Go” as your preferred programming language</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Select “GoBOT” as your preferred framework</t>
+  </si>
+  <si>
+    <t>Locate the Ruby programming option.</t>
+  </si>
+  <si>
+    <t>Next, select and view a Java Stream</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>Navigate to the GoLang competitive coding lobby.</t>
+  </si>
+  <si>
+    <t>Identify the users participating in the competition.</t>
+  </si>
+  <si>
+    <t>Read out the third question in the comments section.</t>
+  </si>
+  <si>
+    <t>The users all found the UI to be self explainatory. They had issues with the scrolling, but those issues are likely due to our improvised screen sharing software from Zoom. There were moments where one of the users was confused by the expanding and minimizing of the comment section, both from not seeing the results right away and by having the screen snap back up. They all liked the registration section. One user noted that the drop down menus could be opened at any time, but could not be closed again.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,6 +304,13 @@
       <sz val="24"/>
       <color theme="1" tint="0.14999847407452621"/>
       <name val="Calibri (Textkörper)_x0000_"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="10">
@@ -452,7 +486,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -584,6 +618,18 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -609,18 +655,6 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -643,6 +677,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -958,14 +999,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="39" customHeight="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="45"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="48"/>
     </row>
     <row r="2" spans="1:6" ht="19.149999999999999" customHeight="1">
       <c r="A2" s="13"/>
@@ -979,59 +1020,59 @@
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="46">
+      <c r="B5" s="49">
         <v>1</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="4" t="s">
@@ -1065,59 +1106,59 @@
       <c r="A13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="6" t="s">
@@ -41150,6 +41191,12 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="18">
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B3:F3"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="E18:F18"/>
@@ -41162,12 +41209,6 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="E16:F16"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="93" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -41181,7 +41222,7 @@
   </sheetPr>
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="B11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="M24" sqref="M24:P24"/>
     </sheetView>
   </sheetViews>
@@ -41848,10 +41889,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="C11" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24:P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -41942,39 +41983,99 @@
       <c r="G4" s="32"/>
     </row>
     <row r="5" spans="1:16">
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="C5" s="31"/>
       <c r="D5" s="32"/>
       <c r="E5" s="32"/>
       <c r="F5" s="33"/>
       <c r="G5" s="32"/>
+      <c r="M5" s="1">
+        <v>5</v>
+      </c>
+      <c r="N5" s="1">
+        <v>5</v>
+      </c>
+      <c r="O5" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:16">
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="C6" s="31"/>
       <c r="D6" s="32"/>
       <c r="E6" s="32"/>
       <c r="F6" s="33"/>
       <c r="G6" s="32"/>
+      <c r="M6" s="1">
+        <v>5</v>
+      </c>
+      <c r="N6" s="1">
+        <v>5</v>
+      </c>
+      <c r="O6" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:16">
+      <c r="B7" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="C7" s="31"/>
       <c r="D7" s="32"/>
       <c r="E7" s="32"/>
       <c r="F7" s="33"/>
       <c r="G7" s="32"/>
+      <c r="M7" s="1">
+        <v>5</v>
+      </c>
+      <c r="N7" s="1">
+        <v>5</v>
+      </c>
+      <c r="O7" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:16">
+      <c r="B8" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="C8" s="31"/>
       <c r="D8" s="32"/>
       <c r="E8" s="32"/>
       <c r="F8" s="33"/>
       <c r="G8" s="32"/>
+      <c r="M8" s="1">
+        <v>5</v>
+      </c>
+      <c r="N8" s="1">
+        <v>5</v>
+      </c>
+      <c r="O8" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:16">
+      <c r="B9" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="C9" s="31"/>
       <c r="D9" s="32"/>
       <c r="E9" s="32"/>
       <c r="F9" s="33"/>
       <c r="G9" s="32"/>
+      <c r="M9" s="1">
+        <v>5</v>
+      </c>
+      <c r="N9" s="1">
+        <v>5</v>
+      </c>
+      <c r="O9" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:16">
       <c r="C10" s="31"/>
@@ -41996,27 +42097,63 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="15"/>
+      <c r="B12" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="C12" s="31"/>
       <c r="D12" s="32"/>
       <c r="E12" s="32"/>
       <c r="F12" s="33"/>
       <c r="G12" s="32"/>
+      <c r="M12" s="1">
+        <v>5</v>
+      </c>
+      <c r="N12" s="1">
+        <v>5</v>
+      </c>
+      <c r="O12" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="15"/>
+      <c r="B13" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="C13" s="31"/>
       <c r="D13" s="32"/>
       <c r="E13" s="32"/>
       <c r="F13" s="33"/>
       <c r="G13" s="32"/>
+      <c r="M13" s="1">
+        <v>3</v>
+      </c>
+      <c r="N13" s="1">
+        <v>5</v>
+      </c>
+      <c r="O13" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="15"/>
+      <c r="B14" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="C14" s="31"/>
       <c r="D14" s="32"/>
       <c r="E14" s="32"/>
       <c r="F14" s="33"/>
       <c r="G14" s="32"/>
+      <c r="M14" s="1">
+        <v>3</v>
+      </c>
+      <c r="N14" s="1">
+        <v>5</v>
+      </c>
+      <c r="O14" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:16">
       <c r="C15" s="31"/>
@@ -42036,49 +42173,109 @@
       <c r="F16" s="33"/>
       <c r="G16" s="32"/>
     </row>
-    <row r="17" spans="2:13">
+    <row r="17" spans="2:16">
+      <c r="B17" s="58" t="s">
+        <v>37</v>
+      </c>
       <c r="C17" s="31"/>
       <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="33"/>
       <c r="G17" s="32"/>
-    </row>
-    <row r="18" spans="2:13">
+      <c r="M17" s="1">
+        <v>5</v>
+      </c>
+      <c r="N17" s="1">
+        <v>5</v>
+      </c>
+      <c r="O17" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16">
+      <c r="B18" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="C18" s="31"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="33"/>
       <c r="G18" s="32"/>
-    </row>
-    <row r="19" spans="2:13">
+      <c r="M18" s="1">
+        <v>5</v>
+      </c>
+      <c r="N18" s="1">
+        <v>4</v>
+      </c>
+      <c r="O18" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16">
+      <c r="B19" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="C19" s="31"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="33"/>
       <c r="G19" s="32"/>
-    </row>
-    <row r="20" spans="2:13">
+      <c r="M19" s="1">
+        <v>5</v>
+      </c>
+      <c r="N19" s="1">
+        <v>5</v>
+      </c>
+      <c r="O19" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16">
+      <c r="B20" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="C20" s="31"/>
       <c r="D20" s="32"/>
       <c r="E20" s="32"/>
       <c r="F20" s="33"/>
       <c r="G20" s="32"/>
-    </row>
-    <row r="21" spans="2:13">
+      <c r="M20" s="1">
+        <v>5</v>
+      </c>
+      <c r="N20" s="1">
+        <v>5</v>
+      </c>
+      <c r="O20" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16">
+      <c r="B21" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="C21" s="31"/>
       <c r="D21" s="32"/>
       <c r="E21" s="32"/>
       <c r="F21" s="33"/>
       <c r="G21" s="32"/>
-    </row>
-    <row r="22" spans="2:13">
+      <c r="M21" s="1">
+        <v>5</v>
+      </c>
+      <c r="N21" s="1">
+        <v>5</v>
+      </c>
+      <c r="O21" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16">
       <c r="C22" s="31"/>
       <c r="D22" s="32"/>
       <c r="E22" s="32"/>
       <c r="F22" s="33"/>
       <c r="G22" s="32"/>
     </row>
-    <row r="23" spans="2:13">
+    <row r="23" spans="2:16">
       <c r="C23" s="34" t="s">
         <v>53</v>
       </c>
@@ -42093,7 +42290,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="2:13" ht="193.5" customHeight="1">
+    <row r="24" spans="2:16" ht="193.5" customHeight="1">
       <c r="B24" s="22"/>
       <c r="C24" s="52" t="s">
         <v>54</v>
@@ -42102,14 +42299,38 @@
       <c r="E24" s="53"/>
       <c r="F24" s="54"/>
       <c r="G24" s="35"/>
-    </row>
-    <row r="25" spans="2:13">
+      <c r="M24" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="N24" s="59"/>
+      <c r="O24" s="59"/>
+      <c r="P24" s="59"/>
+    </row>
+    <row r="25" spans="2:16">
       <c r="C25" s="21"/>
+      <c r="M25" s="59"/>
+      <c r="N25" s="59"/>
+      <c r="O25" s="59"/>
+      <c r="P25" s="59"/>
+    </row>
+    <row r="26" spans="2:16">
+      <c r="M26" s="59"/>
+      <c r="N26" s="59"/>
+      <c r="O26" s="59"/>
+      <c r="P26" s="59"/>
+    </row>
+    <row r="27" spans="2:16">
+      <c r="M27" s="59"/>
+      <c r="N27" s="59"/>
+      <c r="O27" s="59"/>
+      <c r="P27" s="59"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C24:F24"/>
+    <mergeCell ref="M24:P27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added metrics to excel spreadsheet
</commit_message>
<xml_diff>
--- a/UberCode_FinalProject_TestReport.xlsx
+++ b/UberCode_FinalProject_TestReport.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colton\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Addison Boyer\Documents\Spring 2020\User Interface Design\CSCI443\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8372396D-9936-497A-A1D6-3AA8DE23A8D2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3975" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan Overview" sheetId="1" r:id="rId1"/>
@@ -21,18 +22,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="71">
   <si>
     <t>Testing Scope</t>
   </si>
@@ -240,11 +235,17 @@
   <si>
     <t>The users all found the UI to be self explainatory. They had issues with the scrolling, but those issues are likely due to our improvised screen sharing software from Zoom. There were moments where one of the users was confused by the expanding and minimizing of the comment section, both from not seeing the results right away and by having the screen snap back up. They all liked the registration section. One user noted that the drop down menus could be opened at any time, but could not be closed again.</t>
   </si>
+  <si>
+    <t xml:space="preserve">Overall the testing went well, and most particpants were able to complete the tasks relatively easily. The main pain points were users not being able to find the home button and not understanding what was meant when they were asked to 'report' on what they were seeing. Also, the live coding section was too large and users often didn't realize that they needed to scroll down past that section to find the comments. All of these issues have been addressed in the updated prototype and script that will be used for the second round of testing.  </t>
+  </si>
+  <si>
+    <t>Overall testing seemed to go smoother than last time.  It appeared that users were able to recognize the home button easier.  One user mentioned that the navigation menu should be condensed into a single component, and shouldn't have an over arrow.  One testing participant noticed a typo in the static text in our prototype.  The comments section seemed to be more recognizable when condensed closer to the top of the page.  One user mentioned that it was difficult to tell whether there was content below or not on small screens.  After clicking didn't realize content had popped up.  One user mentioned that instead of having next on the last step of user account creation, have finish.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -618,17 +619,8 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -655,6 +647,18 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -678,9 +682,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -976,7 +977,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF43A666"/>
     <pageSetUpPr fitToPage="1"/>
@@ -987,28 +988,28 @@
       <selection activeCell="E15" sqref="E15:F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.88671875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="36.5703125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="13.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="36.5546875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="39" customHeight="1">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="48"/>
-    </row>
-    <row r="2" spans="1:6" ht="19.149999999999999" customHeight="1">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="46"/>
+    </row>
+    <row r="2" spans="1:6" ht="19.2" customHeight="1">
       <c r="A2" s="13"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -1020,59 +1021,59 @@
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="49">
+      <c r="B5" s="47">
         <v>1</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="4" t="s">
@@ -1106,59 +1107,59 @@
       <c r="A13" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="6" t="s">
@@ -41191,12 +41192,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="18">
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B3:F3"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="E18:F18"/>
@@ -41209,6 +41204,12 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="E16:F16"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="93" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -41216,28 +41217,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF2E6AB2"/>
   </sheetPr>
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView topLeftCell="B11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24:P24"/>
+    <sheetView topLeftCell="B17" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5:N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="78.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="4.85546875" style="1" customWidth="1"/>
-    <col min="8" max="11" width="8.85546875" style="1"/>
-    <col min="12" max="12" width="3.7109375" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="15.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="78.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="4.88671875" style="1" customWidth="1"/>
+    <col min="8" max="11" width="8.88671875" style="1"/>
+    <col min="12" max="12" width="3.6640625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -41850,26 +41851,26 @@
     </row>
     <row r="24" spans="2:16" ht="193.5" customHeight="1">
       <c r="B24" s="22"/>
-      <c r="C24" s="52" t="s">
+      <c r="C24" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="55" t="s">
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="H24" s="56"/>
-      <c r="I24" s="56"/>
-      <c r="J24" s="56"/>
-      <c r="K24" s="56"/>
-      <c r="L24" s="56"/>
-      <c r="M24" s="57" t="s">
+      <c r="H24" s="57"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="57"/>
+      <c r="L24" s="57"/>
+      <c r="M24" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="N24" s="57"/>
-      <c r="O24" s="57"/>
-      <c r="P24" s="57"/>
+      <c r="N24" s="58"/>
+      <c r="O24" s="58"/>
+      <c r="P24" s="58"/>
     </row>
     <row r="25" spans="2:16">
       <c r="C25" s="21"/>
@@ -41885,28 +41886,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C11" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24:P27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="78.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="4.85546875" style="1" customWidth="1"/>
-    <col min="8" max="11" width="8.85546875" style="1"/>
-    <col min="12" max="12" width="3.7109375" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="15.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="78.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="4.88671875" style="1" customWidth="1"/>
+    <col min="8" max="11" width="8.88671875" style="1"/>
+    <col min="12" max="12" width="3.6640625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -41991,6 +41992,15 @@
       <c r="E5" s="32"/>
       <c r="F5" s="33"/>
       <c r="G5" s="32"/>
+      <c r="H5" s="1">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1">
+        <v>5</v>
+      </c>
       <c r="M5" s="1">
         <v>5</v>
       </c>
@@ -42010,6 +42020,15 @@
       <c r="E6" s="32"/>
       <c r="F6" s="33"/>
       <c r="G6" s="32"/>
+      <c r="H6" s="1">
+        <v>5</v>
+      </c>
+      <c r="I6" s="1">
+        <v>5</v>
+      </c>
+      <c r="J6" s="1">
+        <v>5</v>
+      </c>
       <c r="M6" s="1">
         <v>5</v>
       </c>
@@ -42029,6 +42048,15 @@
       <c r="E7" s="32"/>
       <c r="F7" s="33"/>
       <c r="G7" s="32"/>
+      <c r="H7" s="1">
+        <v>5</v>
+      </c>
+      <c r="I7" s="1">
+        <v>5</v>
+      </c>
+      <c r="J7" s="1">
+        <v>5</v>
+      </c>
       <c r="M7" s="1">
         <v>5</v>
       </c>
@@ -42048,6 +42076,15 @@
       <c r="E8" s="32"/>
       <c r="F8" s="33"/>
       <c r="G8" s="32"/>
+      <c r="H8" s="1">
+        <v>5</v>
+      </c>
+      <c r="I8" s="1">
+        <v>5</v>
+      </c>
+      <c r="J8" s="1">
+        <v>5</v>
+      </c>
       <c r="M8" s="1">
         <v>5</v>
       </c>
@@ -42067,6 +42104,15 @@
       <c r="E9" s="32"/>
       <c r="F9" s="33"/>
       <c r="G9" s="32"/>
+      <c r="H9" s="1">
+        <v>5</v>
+      </c>
+      <c r="I9" s="1">
+        <v>3</v>
+      </c>
+      <c r="J9" s="1">
+        <v>5</v>
+      </c>
       <c r="M9" s="1">
         <v>5</v>
       </c>
@@ -42105,6 +42151,15 @@
       <c r="E12" s="32"/>
       <c r="F12" s="33"/>
       <c r="G12" s="32"/>
+      <c r="H12" s="1">
+        <v>5</v>
+      </c>
+      <c r="I12" s="1">
+        <v>5</v>
+      </c>
+      <c r="J12" s="1">
+        <v>5</v>
+      </c>
       <c r="M12" s="1">
         <v>5</v>
       </c>
@@ -42125,6 +42180,15 @@
       <c r="E13" s="32"/>
       <c r="F13" s="33"/>
       <c r="G13" s="32"/>
+      <c r="H13" s="1">
+        <v>5</v>
+      </c>
+      <c r="I13" s="1">
+        <v>5</v>
+      </c>
+      <c r="J13" s="1">
+        <v>5</v>
+      </c>
       <c r="M13" s="1">
         <v>3</v>
       </c>
@@ -42145,6 +42209,15 @@
       <c r="E14" s="32"/>
       <c r="F14" s="33"/>
       <c r="G14" s="32"/>
+      <c r="H14" s="1">
+        <v>5</v>
+      </c>
+      <c r="I14" s="1">
+        <v>5</v>
+      </c>
+      <c r="J14" s="1">
+        <v>5</v>
+      </c>
       <c r="M14" s="1">
         <v>3</v>
       </c>
@@ -42174,7 +42247,7 @@
       <c r="G16" s="32"/>
     </row>
     <row r="17" spans="2:16">
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="42" t="s">
         <v>37</v>
       </c>
       <c r="C17" s="31"/>
@@ -42182,6 +42255,15 @@
       <c r="E17" s="32"/>
       <c r="F17" s="33"/>
       <c r="G17" s="32"/>
+      <c r="H17" s="1">
+        <v>5</v>
+      </c>
+      <c r="I17" s="1">
+        <v>5</v>
+      </c>
+      <c r="J17" s="1">
+        <v>5</v>
+      </c>
       <c r="M17" s="1">
         <v>5</v>
       </c>
@@ -42201,6 +42283,15 @@
       <c r="E18" s="32"/>
       <c r="F18" s="33"/>
       <c r="G18" s="32"/>
+      <c r="H18" s="1">
+        <v>5</v>
+      </c>
+      <c r="I18" s="1">
+        <v>3</v>
+      </c>
+      <c r="J18" s="1">
+        <v>5</v>
+      </c>
       <c r="M18" s="1">
         <v>5</v>
       </c>
@@ -42220,6 +42311,15 @@
       <c r="E19" s="32"/>
       <c r="F19" s="33"/>
       <c r="G19" s="32"/>
+      <c r="H19" s="1">
+        <v>5</v>
+      </c>
+      <c r="I19" s="1">
+        <v>5</v>
+      </c>
+      <c r="J19" s="1">
+        <v>5</v>
+      </c>
       <c r="M19" s="1">
         <v>5</v>
       </c>
@@ -42239,6 +42339,15 @@
       <c r="E20" s="32"/>
       <c r="F20" s="33"/>
       <c r="G20" s="32"/>
+      <c r="H20" s="1">
+        <v>5</v>
+      </c>
+      <c r="I20" s="1">
+        <v>5</v>
+      </c>
+      <c r="J20" s="1">
+        <v>5</v>
+      </c>
       <c r="M20" s="1">
         <v>5</v>
       </c>
@@ -42258,6 +42367,15 @@
       <c r="E21" s="32"/>
       <c r="F21" s="33"/>
       <c r="G21" s="32"/>
+      <c r="H21" s="1">
+        <v>5</v>
+      </c>
+      <c r="I21" s="1">
+        <v>5</v>
+      </c>
+      <c r="J21" s="1">
+        <v>5</v>
+      </c>
       <c r="M21" s="1">
         <v>5</v>
       </c>
@@ -42292,13 +42410,19 @@
     </row>
     <row r="24" spans="2:16" ht="193.5" customHeight="1">
       <c r="B24" s="22"/>
-      <c r="C24" s="52" t="s">
-        <v>54</v>
+      <c r="C24" s="53" t="s">
+        <v>69</v>
       </c>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="55"/>
       <c r="G24" s="35"/>
+      <c r="H24" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="I24" s="54"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="55"/>
       <c r="M24" s="59" t="s">
         <v>68</v>
       </c>
@@ -42326,9 +42450,10 @@
       <c r="P27" s="59"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C24:F24"/>
     <mergeCell ref="M24:P27"/>
+    <mergeCell ref="H24:K24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>